<commit_message>
commit the current work
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/List_of_Player.xlsx
+++ b/Manipulating Excels with Code/List_of_Player.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comet\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF11394-813F-4897-A22A-96B9A181C006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467985C2-15B2-4C2E-BAAE-F3150DA6F289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30195" yWindow="4125" windowWidth="19830" windowHeight="14970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <t>Béa</t>
   </si>
   <si>
-    <t>CACA</t>
+    <t>Hugo D</t>
   </si>
 </sst>
 </file>
@@ -369,7 +369,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added the Elimination still have issues with the datetime
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/List_of_Player.xlsx
+++ b/Manipulating Excels with Code/List_of_Player.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comet\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467985C2-15B2-4C2E-BAAE-F3150DA6F289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7446FB4C-99B2-4764-A3E7-7ADEFB613697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Joueur</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Hugo D</t>
+  </si>
+  <si>
+    <t>Mathieu</t>
   </si>
 </sst>
 </file>
@@ -366,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -414,6 +417,11 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added the possibility for Didier to specify his killer
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/List_of_Player.xlsx
+++ b/Manipulating Excels with Code/List_of_Player.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comet\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7446FB4C-99B2-4764-A3E7-7ADEFB613697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE56CC9-FC8E-4E89-BDB5-C9846F8D5545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19320" yWindow="5040" windowWidth="21870" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Joueur</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Mathieu</t>
+  </si>
+  <si>
+    <t>Anne-Lise</t>
+  </si>
+  <si>
+    <t>Jean Rob</t>
   </si>
 </sst>
 </file>
@@ -369,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,6 +428,16 @@
         <v>8</v>
       </c>
     </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>